<commit_message>
Add a new method to TestData class.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TopNav" sheetId="1" r:id="rId1"/>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>L6Y 0Z1</t>
+  </si>
+  <si>
+    <t>Order ID</t>
   </si>
 </sst>
 </file>
@@ -503,8 +506,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1:B8"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -562,7 +565,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0">
         <v>1216464018</v>

</xml_diff>

<commit_message>
Used getData method to replace hardcoded testdata values
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Samsung_T5/bay/TestData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B98AE8-60B8-074E-BC3A-5F6605370C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="18200" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TopNav" sheetId="1" r:id="rId1"/>
-    <sheet name="TestInputs" sheetId="2" r:id="rId5"/>
+    <sheet name="TestInputs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>WOMEN</t>
   </si>
@@ -47,9 +53,6 @@
     <t>ZELLERS</t>
   </si>
   <si>
-    <t xml:space="preserve">Search String </t>
-  </si>
-  <si>
     <t>towel</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
     <t>Cushions</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>Postal Code</t>
   </si>
   <si>
@@ -93,25 +93,25 @@
   </si>
   <si>
     <t>Order ID</t>
+  </si>
+  <si>
+    <t>mango women</t>
+  </si>
+  <si>
+    <t>Search String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="JetBrains Mono"/>
-      <color rgb="FF6AAB73"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,11 +134,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0">
-      <alignment/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,6 +145,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -196,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,9 +229,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,6 +281,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,62 +473,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -504,79 +538,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>12</v>
       </c>
       <c r="B2">
         <v>600086722740</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>1216464018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="0">
-        <v>1216464018</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed blank space at the end in "Search String" from TestData.xlsx file. ColumnCount counter in getData method was starting from column 0, so our inputData array also included the key value. Fixed this by starting the counter from 1. Updated SmokeTests to use index 0 for getting data.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -94,12 +94,15 @@
   <si>
     <t>Order ID</t>
   </si>
+  <si>
+    <t>Search String</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +116,11 @@
       <color rgb="FF6AAB73"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -122,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,14 +138,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,7 +462,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -507,14 +526,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="13.1406" customWidth="1"/>
+    <col min="2" max="2" width="11.4258" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -567,7 +590,7 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7" s="2">
         <v>1216464018</v>
       </c>
     </row>
@@ -575,7 +598,7 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the Search String that got removed in TestData.xlsx Corrected the index for autosuggestionSearch test.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Search String</t>
+  </si>
+  <si>
+    <t>mango women</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,6 +545,9 @@
       <c r="B1" t="s">
         <v>11</v>
       </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">

</xml_diff>